<commit_message>
Went through all the specs should be done now
Lets cross our fingers should be 'A' quality work
</commit_message>
<xml_diff>
--- a/Assignment One/AnswerChecker.xlsx
+++ b/Assignment One/AnswerChecker.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="13395" windowHeight="9015"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -231,21 +231,9 @@
     <t>black</t>
   </si>
   <si>
-    <t>thecube thebox theglass thecup thetube thedish theblockA theblockB theblockC theblockD theblockE thepencil</t>
-  </si>
-  <si>
-    <t>thedish</t>
-  </si>
-  <si>
-    <t>thebaseball theballoon</t>
-  </si>
-  <si>
     <t>thetable theblockA theblockB theblockC</t>
   </si>
   <si>
-    <t>thetube theblockA</t>
-  </si>
-  <si>
     <t>theball</t>
   </si>
   <si>
@@ -276,9 +264,6 @@
     <t xml:space="preserve">thecube </t>
   </si>
   <si>
-    <t xml:space="preserve">themarble therock theglass thetube thepencil </t>
-  </si>
-  <si>
     <t xml:space="preserve">thedish </t>
   </si>
   <si>
@@ -288,15 +273,9 @@
     <t xml:space="preserve">Nothing </t>
   </si>
   <si>
-    <t xml:space="preserve">thecube thebox theglass thecup thetube thedish theblockA theblockB theblockC theblockD theblockE thepencil </t>
-  </si>
-  <si>
     <t xml:space="preserve">theblockA theblockB theblockC theblockD theblockE thepencil </t>
   </si>
   <si>
-    <t xml:space="preserve">thebaseball theballoon </t>
-  </si>
-  <si>
     <t xml:space="preserve">robbie theprism thecube themarble thebaseball therock theball thedish theblockA theblockB theblockC theblockD thepencil theballoon </t>
   </si>
   <si>
@@ -306,9 +285,6 @@
     <t xml:space="preserve">theball theballoon theblockA theblockB theblockC theblockD theblockE thedish thepencil thetube </t>
   </si>
   <si>
-    <t xml:space="preserve">thebox thetube </t>
-  </si>
-  <si>
     <t xml:space="preserve">robbie thetable thecube thebaseball thebox therock thecup thetube theball theblockA theblockB theblockC theblockD theblockE thepencil theballoon </t>
   </si>
   <si>
@@ -318,9 +294,6 @@
     <t xml:space="preserve">thetable theblockA theblockB theblockC </t>
   </si>
   <si>
-    <t xml:space="preserve">thetube theblockA </t>
-  </si>
-  <si>
     <t xml:space="preserve">theblockA theblockB theblockC theblockD thecube thedish </t>
   </si>
   <si>
@@ -345,9 +318,6 @@
     <t xml:space="preserve">thebaseball thecube thecup therock theblockA thetube </t>
   </si>
   <si>
-    <t>Nothing</t>
-  </si>
-  <si>
     <t>Total Wrong</t>
   </si>
   <si>
@@ -357,14 +327,44 @@
     <t xml:space="preserve">thebox theglass thecup thetube theballoon  </t>
   </si>
   <si>
-    <t xml:space="preserve">robbie thetable thecube thebox thetube theblockA theblockB theblockC theblockD theblockE thepencil </t>
+    <t xml:space="preserve">robbie thetable thecube thebox </t>
+  </si>
+  <si>
+    <t xml:space="preserve">themarble therock thepencil </t>
+  </si>
+  <si>
+    <t xml:space="preserve">theglass thecup thetube thedish </t>
+  </si>
+  <si>
+    <t xml:space="preserve">thetube </t>
+  </si>
+  <si>
+    <t xml:space="preserve">thetube theball theblockA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">theblockA theblockB theblockC theblockD thecube thedish  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">robbie thetable thecube thedish theblockA theblockB theblockC theblockD  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">robbie thetable thecube thebox thetube theblockA theblockB theblockC theblockD theblockE thepencil  </t>
+  </si>
+  <si>
+    <t>cube</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thecube thebox theblockA theblockB theblockC theblockD theblockE theglass thecup thetube thepencil thedish </t>
+  </si>
+  <si>
+    <t xml:space="preserve">theblockA theblockB theblockC theblockD thecube  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,7 +402,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -425,21 +425,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -538,7 +528,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -573,7 +562,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -749,14 +737,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="61.5703125" style="1" customWidth="1"/>
@@ -768,7 +756,7 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="18" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
@@ -785,10 +773,10 @@
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -810,7 +798,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -828,7 +816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -846,10 +834,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -871,7 +859,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -889,7 +877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -907,10 +895,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -932,7 +920,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -950,7 +938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -968,10 +956,10 @@
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -993,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1011,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1019,20 +1007,20 @@
         <v>13</v>
       </c>
       <c r="C13" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1054,7 +1042,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1072,7 +1060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1090,7 +1078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1108,7 +1096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1126,7 +1114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1144,7 +1132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1162,7 +1150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1180,7 +1168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1198,7 +1186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1216,7 +1204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1234,7 +1222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1252,7 +1240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1270,7 +1258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1288,7 +1276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1306,7 +1294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1324,7 +1312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1342,10 +1330,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1353,17 +1341,17 @@
         <v>31</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E32" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1371,7 +1359,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>68</v>
@@ -1381,7 +1369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="52.5" customHeight="1">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1389,17 +1377,17 @@
         <v>33</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="E34" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="51" customHeight="1">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1407,17 +1395,17 @@
         <v>34</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="E35" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1435,7 +1423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1443,7 +1431,7 @@
         <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>70</v>
@@ -1453,7 +1441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="105" customHeight="1">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1461,17 +1449,17 @@
         <v>37</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>69</v>
+        <v>111</v>
       </c>
       <c r="E38" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="100.5" customHeight="1">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1479,17 +1467,17 @@
         <v>38</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>71</v>
+        <v>112</v>
       </c>
       <c r="E39" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="70.5" customHeight="1">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1497,17 +1485,17 @@
         <v>39</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E40" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="47.25" customHeight="1">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1515,17 +1503,17 @@
         <v>40</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E41" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="49.5" customHeight="1">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1533,17 +1521,17 @@
         <v>41</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="E42" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="96.75" customHeight="1">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1551,17 +1539,17 @@
         <v>42</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E43" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1569,7 +1557,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>69</v>
@@ -1579,7 +1567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="98.25" customHeight="1">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1587,17 +1575,17 @@
         <v>44</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E45" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1605,17 +1593,17 @@
         <v>45</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="E46" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="131.25" customHeight="1">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1623,17 +1611,17 @@
         <v>46</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E47" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="49.5" customHeight="1">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1641,17 +1629,17 @@
         <v>47</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="E48" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="60" customHeight="1">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1659,17 +1647,17 @@
         <v>48</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E49" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="30">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1677,17 +1665,17 @@
         <v>49</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E50" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1695,17 +1683,17 @@
         <v>50</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="E51" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="69" customHeight="1">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1713,17 +1701,17 @@
         <v>51</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E52" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1731,7 +1719,7 @@
         <v>52</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>69</v>
@@ -1741,7 +1729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="83.25" customHeight="1">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1749,17 +1737,17 @@
         <v>53</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="E54" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="139.5" customHeight="1">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1767,17 +1755,17 @@
         <v>54</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E55" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="97.5" customHeight="1">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1785,17 +1773,17 @@
         <v>55</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E56" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1803,7 +1791,7 @@
         <v>56</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>69</v>
@@ -1813,7 +1801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1821,7 +1809,7 @@
         <v>57</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>69</v>
@@ -1831,7 +1819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -1839,17 +1827,17 @@
         <v>58</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E59" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="122.25" customHeight="1">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -1857,17 +1845,17 @@
         <v>59</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="E60" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -1875,17 +1863,17 @@
         <v>60</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E61" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="129.75" customHeight="1">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -1893,17 +1881,17 @@
         <v>61</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E62" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="69.75" customHeight="1">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -1911,17 +1899,17 @@
         <v>62</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E63" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="101.25" customHeight="1">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -1929,17 +1917,17 @@
         <v>63</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E64" s="1" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="84.75" customHeight="1">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -1947,10 +1935,10 @@
         <v>64</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E65" s="1" t="b">
         <f t="shared" si="0"/>
@@ -1959,12 +1947,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E30 E32:E1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1973,24 +1961,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>